<commit_message>
Add date filtering, unassigned job reasons, technician views, and Koyeb deployment guides
Features added:
- Date filter on assignment page to view all jobs for selected date
- Unassigned job reasons display (skill mismatch, time window, capacity)
- Admin technician view with assignments, map, and timeline
- Service request admin table shows date and time window columns
- Fixed time window validation (check if technician arrives within window)
- Sample data generator updated for Nov 1, 2025 with tight windows

Koyeb deployment:
- Added DEPLOY_KOYEB_ADMIN.md comprehensive guide
- Added QUICK_DEPLOY.md quick reference
- Added create_admin management command for easy admin user creation
- Updated Excel sample data with Nov 1, 2025 dates

Bug fixes:
- Fixed date serialization in session storage
- Fixed date filter to show all jobs (pending + assigned) for selected date
- Fixed technician arrival time window validation logic
</commit_message>
<xml_diff>
--- a/sample_data_50_people.xlsx
+++ b/sample_data_50_people.xlsx
@@ -533,12 +533,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>tech_blake</t>
+          <t>tech_morgan</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>tech.blake@company.com</t>
+          <t>tech.morgan@company.com</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -548,7 +548,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0448030357</t>
+          <t>0462965398</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
@@ -560,47 +560,47 @@
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
-          <t>558 Chapel Street, South Yarra VIC 3141</t>
+          <t>63 Rathdowne Street, Carlton VIC 3053</t>
         </is>
       </c>
       <c r="N2" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>06:00</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Plumbing, Cleaning</t>
+          <t>Gas, HVAC, Plumbing</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>#4285F4</t>
+          <t>#FBBC05</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Customer</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>tech_dakota</t>
+          <t>emily_clark</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>tech.dakota@company.com</t>
+          <t>emily.clark@example.com</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -610,59 +610,63 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0442190869</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>244 Swan Street, Richmond VIC 3121</t>
-        </is>
-      </c>
-      <c r="N3" t="n">
-        <v>8</v>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>09:00</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>18:00</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>HVAC, Plumbing</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>#34A853</t>
-        </is>
-      </c>
+          <t>0456011717</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>944 Nicholson Street, Footscray VIC 3011</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>90</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2025-11-01 10:00</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2025-11-01 12:00</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Electric</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Appliance Installation</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Customer</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>sarah_brown</t>
+          <t>tech_jamie</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>sarah.brown@example.com</t>
+          <t>tech.jamie@company.com</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -672,63 +676,59 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0465729817</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>439 Fitzroy Street, St Kilda VIC 3182</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>60</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>2025-11-02 09:00</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>2025-11-02 11:00</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Gas</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>Gas Leak Repair</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
+          <t>0481895582</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>706 Nicholson Street, Footscray VIC 3011</t>
+        </is>
+      </c>
+      <c r="N4" t="n">
+        <v>6</v>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>Electric, Plumbing, Security</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>#4285F4</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Customer</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>evelyn_thompson</t>
+          <t>tech_cameron</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>evelyn.thompson@example.com</t>
+          <t>tech.cameron@company.com</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -738,48 +738,44 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0449698926</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>243 Nicholson Street, Footscray VIC 3011</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>120</v>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>2025-11-05 09:00</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>2025-11-05 13:00</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Gas</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>Gas Leak Repair</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="inlineStr"/>
+          <t>0496250839</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>255 Springvale Road, Mulgrave VIC 3170</t>
+        </is>
+      </c>
+      <c r="N5" t="n">
+        <v>8</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>06:00</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>Plumbing, Gas, Carpentry</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>#EA4335</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -789,12 +785,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>sofia_walker</t>
+          <t>mark_robinson</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>sofia.walker@example.com</t>
+          <t>mark.robinson@example.com</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -804,40 +800,40 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0423206814</t>
+          <t>0439676172</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>71 Dandenong Railway Station, Dandenong VIC 3175</t>
+          <t>147 Swan Street, Richmond VIC 3121</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-10-31 12:00</t>
+          <t>2025-11-01 14:00</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>2025-10-31 16:00</t>
+          <t>2025-11-01 16:00</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Security</t>
+          <t>IT</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Safety Inspection</t>
+          <t>System Upgrade</t>
         </is>
       </c>
       <c r="M6" t="inlineStr"/>
@@ -850,17 +846,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Customer</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>donald_young</t>
+          <t>tech_sage</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>donald.young@example.com</t>
+          <t>tech.sage@company.com</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -870,48 +866,44 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0499016918</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>436 Mulgrave Business Park, Mulgrave VIC 3170</t>
-        </is>
-      </c>
-      <c r="G7" t="n">
-        <v>90</v>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>2025-11-02 13:00</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>2025-11-02 16:00</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>HVAC</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>HVAC Maintenance</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr"/>
+          <t>0486252294</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>968 Rathdowne Street, Carlton VIC 3053</t>
+        </is>
+      </c>
+      <c r="N7" t="n">
+        <v>5</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>IT, Security</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>#EA4335</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -921,12 +913,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>victoria_wright</t>
+          <t>sarah_brown</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>victoria.wright@example.com</t>
+          <t>sarah.brown@example.com</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -936,40 +928,40 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0478842094</t>
+          <t>0462705300</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>222 Fitzroy Street, St Kilda VIC 3182</t>
+          <t>800 Ferntree Gully Road, Mulgrave VIC 3170</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-11-02 12:00</t>
+          <t>2025-11-01 14:00</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>2025-11-02 14:00</t>
+          <t>2025-11-01 15:00</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Electric</t>
+          <t>IT</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Appliance Installation</t>
+          <t>System Upgrade</t>
         </is>
       </c>
       <c r="M8" t="inlineStr"/>
@@ -982,17 +974,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Customer</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>tech_avery</t>
+          <t>charlotte_thomas</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>tech.avery@company.com</t>
+          <t>charlotte.thomas@example.com</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1002,59 +994,63 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0458511012</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>597 Bridge Road, Richmond VIC 3121</t>
-        </is>
-      </c>
-      <c r="N9" t="n">
-        <v>8</v>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>08:00</t>
-        </is>
-      </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>Roofing, Carpentry, Cleaning</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>#4285F4</t>
-        </is>
-      </c>
+          <t>0440744539</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>940 Commercial Road, South Yarra VIC 3141</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>120</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2025-11-01 10:00</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>2025-11-01 11:00</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Plumbing</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Emergency Callout</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Customer</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>paul_scott</t>
+          <t>tech_reese</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>paul.scott@example.com</t>
+          <t>tech.reese@company.com</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1064,63 +1060,59 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0442674074</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>925 Nicholson Street, Footscray VIC 3011</t>
-        </is>
-      </c>
-      <c r="G10" t="n">
-        <v>180</v>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>2025-10-31 09:00</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>2025-10-31 12:00</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>Electric</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>Maintenance Check</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr"/>
+          <t>0462996689</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>364 Derrimut Road, Tarneit VIC 3029</t>
+        </is>
+      </c>
+      <c r="N10" t="n">
+        <v>6</v>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>Electric, Solar, HVAC, IT</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>#FBBC05</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Customer</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>david_williams</t>
+          <t>tech_quinn</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>david.williams@example.com</t>
+          <t>tech.quinn@company.com</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1130,48 +1122,44 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0499000073</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>793 Barkly Street, Footscray VIC 3011</t>
-        </is>
-      </c>
-      <c r="G11" t="n">
-        <v>120</v>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>2025-11-03 09:00</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>2025-11-03 13:00</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>Plumbing</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>Routine Service</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="inlineStr"/>
+          <t>0494373117</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>709 Dandenong Railway Station, Dandenong VIC 3175</t>
+        </is>
+      </c>
+      <c r="N11" t="n">
+        <v>5</v>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>Roofing, Carpentry</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>#FF6D01</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1181,12 +1169,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>christopher_lee</t>
+          <t>elizabeth_lewis</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>christopher.lee@example.com</t>
+          <t>elizabeth.lewis@example.com</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1196,25 +1184,25 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>0497886145</t>
+          <t>0480601698</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>29 Barkly Street, Footscray VIC 3011</t>
+          <t>243 Fitzroy Street, St Kilda VIC 3182</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-11-03 13:00</t>
+          <t>2025-11-01 15:00</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>2025-11-03 16:00</t>
+          <t>2025-11-01 17:00</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1224,12 +1212,12 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Emergency Callout</t>
+          <t>Routine Service</t>
         </is>
       </c>
       <c r="M12" t="inlineStr"/>
@@ -1242,17 +1230,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Customer</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>robert_rodriguez</t>
+          <t>tech_jordan</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>robert.rodriguez@example.com</t>
+          <t>tech.jordan@company.com</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1262,48 +1250,44 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>0487868376</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>642 Swanston Street, Melbourne VIC 3000</t>
-        </is>
-      </c>
-      <c r="G13" t="n">
-        <v>180</v>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>2025-11-02 12:00</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>2025-11-02 15:00</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>IT</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>System Upgrade</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="inlineStr"/>
-      <c r="R13" t="inlineStr"/>
+          <t>0474801753</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>433 Lygon Street, Carlton VIC 3053</t>
+        </is>
+      </c>
+      <c r="N13" t="n">
+        <v>5</v>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>06:00</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>Electric, Solar</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>#FF6D01</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1313,12 +1297,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>abigail_harris</t>
+          <t>christopher_lee</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>abigail.harris@example.com</t>
+          <t>christopher.lee@example.com</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1328,40 +1312,40 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>0494456090</t>
+          <t>0472824095</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>847 Rathdowne Street, Carlton VIC 3053</t>
+          <t>89 Derrimut Road, Tarneit VIC 3029</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-11-03 13:00</t>
+          <t>2025-11-01 12:00</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>2025-11-03 16:00</t>
+          <t>2025-11-01 14:00</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>HVAC</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>HVAC Maintenance</t>
+          <t>Gas Leak Repair</t>
         </is>
       </c>
       <c r="M14" t="inlineStr"/>
@@ -1379,12 +1363,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>steven_king</t>
+          <t>robert_rodriguez</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>steven.king@example.com</t>
+          <t>robert.rodriguez@example.com</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1394,12 +1378,12 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>0465291971</t>
+          <t>0468358757</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>58 Chapel Street, South Yarra VIC 3141</t>
+          <t>461 Bridge Road, Richmond VIC 3121</t>
         </is>
       </c>
       <c r="G15" t="n">
@@ -1407,27 +1391,27 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-10-30 12:00</t>
+          <t>2025-11-01 13:00</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>2025-10-30 16:00</t>
+          <t>2025-11-01 15:00</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Security</t>
+          <t>Electric</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Safety Inspection</t>
+          <t>Electrical Fault</t>
         </is>
       </c>
       <c r="M15" t="inlineStr"/>
@@ -1445,12 +1429,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>harper_martin</t>
+          <t>mia_wilson</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>harper.martin@example.com</t>
+          <t>mia.wilson@example.com</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1460,40 +1444,40 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>0434237802</t>
+          <t>0476672201</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>874 Central Road, Clayton VIC 3168</t>
+          <t>317 Springvale Road, Mulgrave VIC 3170</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-10-30 11:00</t>
+          <t>2025-11-01 11:00</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>2025-10-30 14:00</t>
+          <t>2025-11-01 12:00</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Plumbing</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>System Upgrade</t>
+          <t>Routine Service</t>
         </is>
       </c>
       <c r="M16" t="inlineStr"/>
@@ -1506,17 +1490,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Customer</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>tech_sage</t>
+          <t>amelia_moore</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>tech.sage@company.com</t>
+          <t>amelia.moore@example.com</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1526,44 +1510,48 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0444832196</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>240 Bridge Road, Richmond VIC 3121</t>
-        </is>
-      </c>
-      <c r="N17" t="n">
-        <v>8</v>
-      </c>
-      <c r="O17" t="inlineStr">
-        <is>
-          <t>08:00</t>
-        </is>
-      </c>
-      <c r="P17" t="inlineStr">
-        <is>
-          <t>18:00</t>
-        </is>
-      </c>
-      <c r="Q17" t="inlineStr">
-        <is>
-          <t>IT, Security</t>
-        </is>
-      </c>
-      <c r="R17" t="inlineStr">
-        <is>
-          <t>#34A853</t>
-        </is>
-      </c>
+          <t>0497692482</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>86 Clayton Campus, Monash University, Clayton VIC 3168</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>180</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2025-11-01 16:00</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>2025-11-01 18:00</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Plumbing</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Emergency Callout</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr"/>
+      <c r="Q17" t="inlineStr"/>
+      <c r="R17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1573,12 +1561,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>sophia_martinez</t>
+          <t>charles_jackson</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>sophia.martinez@example.com</t>
+          <t>charles.jackson@example.com</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1588,30 +1576,30 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0436273756</t>
+          <t>0493596754</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>299 Commercial Road, South Yarra VIC 3141</t>
+          <t>975 Chapel Street, South Yarra VIC 3141</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-11-02 12:00</t>
+          <t>2025-11-01 08:00</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>2025-11-02 16:00</t>
+          <t>2025-11-01 10:00</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Electric</t>
+          <t>Security</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1621,7 +1609,7 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Maintenance Check</t>
+          <t>Safety Inspection</t>
         </is>
       </c>
       <c r="M18" t="inlineStr"/>
@@ -1634,17 +1622,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Customer</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>tech_casey</t>
+          <t>sofia_walker</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>tech.casey@company.com</t>
+          <t>sofia.walker@example.com</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1654,59 +1642,63 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0410436964</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
-      <c r="L19" t="inlineStr"/>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>819 Princes Highway, Dandenong VIC 3175</t>
-        </is>
-      </c>
-      <c r="N19" t="n">
-        <v>8</v>
-      </c>
-      <c r="O19" t="inlineStr">
-        <is>
-          <t>08:00</t>
-        </is>
-      </c>
-      <c r="P19" t="inlineStr">
-        <is>
-          <t>18:00</t>
-        </is>
-      </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>HVAC, Electric</t>
-        </is>
-      </c>
-      <c r="R19" t="inlineStr">
-        <is>
-          <t>#4285F4</t>
-        </is>
-      </c>
+          <t>0465228749</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>846 Bridge Road, Richmond VIC 3121</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>90</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2025-11-01 13:00</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>2025-11-01 14:00</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Plumbing</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Plumbing Issue</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr"/>
+      <c r="Q19" t="inlineStr"/>
+      <c r="R19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Customer</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>tech_reese</t>
+          <t>anthony_ramirez</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>tech.reese@company.com</t>
+          <t>anthony.ramirez@example.com</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1716,44 +1708,48 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>0432101123</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr"/>
-      <c r="L20" t="inlineStr"/>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>43 Clayton Road, Clayton VIC 3168</t>
-        </is>
-      </c>
-      <c r="N20" t="n">
-        <v>8</v>
-      </c>
-      <c r="O20" t="inlineStr">
-        <is>
-          <t>08:00</t>
-        </is>
-      </c>
-      <c r="P20" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>Electric, Solar, HVAC, IT</t>
-        </is>
-      </c>
-      <c r="R20" t="inlineStr">
-        <is>
-          <t>#FBBC05</t>
-        </is>
-      </c>
+          <t>0446985387</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>813 Dandenong Railway Station, Dandenong VIC 3175</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>120</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2025-11-01 09:00</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>2025-11-01 10:00</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>IT</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>System Upgrade</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr"/>
+      <c r="Q20" t="inlineStr"/>
+      <c r="R20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1763,12 +1759,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>daniel_white</t>
+          <t>john_smith</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>daniel.white@example.com</t>
+          <t>john.smith@example.com</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1778,12 +1774,12 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>0426396632</t>
+          <t>0412924588</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>981 Rathdowne Street, Carlton VIC 3053</t>
+          <t>587 Dohertys Road, Tarneit VIC 3029</t>
         </is>
       </c>
       <c r="G21" t="n">
@@ -1791,27 +1787,27 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2025-11-02 10:00</t>
+          <t>2025-11-01 13:00</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>2025-11-02 14:00</t>
+          <t>2025-11-01 14:00</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Electric</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>System Upgrade</t>
+          <t>Electrical Fault</t>
         </is>
       </c>
       <c r="M21" t="inlineStr"/>
@@ -1824,17 +1820,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Customer</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>tech_quinn</t>
+          <t>steven_king</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>tech.quinn@company.com</t>
+          <t>steven.king@example.com</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1844,44 +1840,48 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>0439806512</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
-      <c r="K22" t="inlineStr"/>
-      <c r="L22" t="inlineStr"/>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>827 Commercial Road, South Yarra VIC 3141</t>
-        </is>
-      </c>
-      <c r="N22" t="n">
-        <v>8</v>
-      </c>
-      <c r="O22" t="inlineStr">
-        <is>
-          <t>09:00</t>
-        </is>
-      </c>
-      <c r="P22" t="inlineStr">
-        <is>
-          <t>18:00</t>
-        </is>
-      </c>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>Roofing, Carpentry</t>
-        </is>
-      </c>
-      <c r="R22" t="inlineStr">
-        <is>
-          <t>#FF6D01</t>
-        </is>
-      </c>
+          <t>0444593646</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>16 Fitzroy Street, St Kilda VIC 3182</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>90</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2025-11-01 13:00</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>2025-11-01 15:00</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Gas</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>Gas Leak Repair</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr"/>
+      <c r="Q22" t="inlineStr"/>
+      <c r="R22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1891,12 +1891,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>tech_alex</t>
+          <t>tech_casey</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>tech.alex@company.com</t>
+          <t>tech.casey@company.com</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1906,7 +1906,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0482052647</t>
+          <t>0458791764</t>
         </is>
       </c>
       <c r="F23" t="inlineStr"/>
@@ -1918,15 +1918,15 @@
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr">
         <is>
-          <t>922 Nicholson Street, Footscray VIC 3011</t>
+          <t>775 Derrimut Road, Tarneit VIC 3029</t>
         </is>
       </c>
       <c r="N23" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -1936,12 +1936,12 @@
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>Plumbing, Gas</t>
+          <t>HVAC, Electric</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
         <is>
-          <t>#4285F4</t>
+          <t>#FF6D01</t>
         </is>
       </c>
     </row>
@@ -1953,12 +1953,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>mary_johnson</t>
+          <t>richard_gonzalez</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>mary.johnson@example.com</t>
+          <t>richard.gonzalez@example.com</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1968,40 +1968,40 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>0437654557</t>
+          <t>0467607024</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>846 Ferntree Gully Road, Mulgrave VIC 3170</t>
+          <t>640 Tarneit Road, Tarneit VIC 3029</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2025-11-01 12:00</t>
+          <t>2025-11-01 14:00</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>2025-11-01 14:00</t>
+          <t>2025-11-01 15:00</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>HVAC</t>
+          <t>IT</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>HVAC Maintenance</t>
+          <t>System Upgrade</t>
         </is>
       </c>
       <c r="M24" t="inlineStr"/>
@@ -2019,12 +2019,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>thomas_taylor</t>
+          <t>james_miller</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>thomas.taylor@example.com</t>
+          <t>james.miller@example.com</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -2034,40 +2034,40 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>0471773704</t>
+          <t>0493018531</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>873 Lygon Street, Carlton VIC 3053</t>
+          <t>667 Bourke Street, Melbourne VIC 3000</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2025-10-31 11:00</t>
+          <t>2025-11-01 09:00</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>2025-10-31 15:00</t>
+          <t>2025-11-01 11:00</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Plumbing</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Plumbing Issue</t>
+          <t>Gas Leak Repair</t>
         </is>
       </c>
       <c r="M25" t="inlineStr"/>
@@ -2085,12 +2085,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>michael_jones</t>
+          <t>joseph_anderson</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>michael.jones@example.com</t>
+          <t>joseph.anderson@example.com</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2100,20 +2100,20 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>0427134284</t>
+          <t>0463347946</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>991 Ferntree Gully Road, Mulgrave VIC 3170</t>
+          <t>806 Springvale Road, Mulgrave VIC 3170</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2025-11-01 10:00</t>
+          <t>2025-11-01 11:00</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -2123,17 +2123,17 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Security</t>
+          <t>Electric</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Safety Inspection</t>
+          <t>Appliance Installation</t>
         </is>
       </c>
       <c r="M26" t="inlineStr"/>
@@ -2151,12 +2151,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>anthony_ramirez</t>
+          <t>victoria_wright</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>anthony.ramirez@example.com</t>
+          <t>victoria.wright@example.com</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2166,40 +2166,40 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>0490939489</t>
+          <t>0480182314</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>501 Swan Street, Richmond VIC 3121</t>
+          <t>840 Clayton Road, Clayton VIC 3168</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2025-11-01 12:00</t>
+          <t>2025-11-01 11:00</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>2025-11-01 15:00</t>
+          <t>2025-11-01 13:00</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>HVAC</t>
+          <t>Electric</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>High</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>HVAC Maintenance</t>
+          <t>Maintenance Check</t>
         </is>
       </c>
       <c r="M27" t="inlineStr"/>
@@ -2212,17 +2212,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Customer</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>mia_wilson</t>
+          <t>tech_alex</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>mia.wilson@example.com</t>
+          <t>tech.alex@company.com</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2232,48 +2232,44 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>0444192845</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>104 Bourke Street, Melbourne VIC 3000</t>
-        </is>
-      </c>
-      <c r="G28" t="n">
-        <v>180</v>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>2025-10-30 14:00</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>2025-10-30 17:00</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>Security</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>Safety Inspection</t>
-        </is>
-      </c>
-      <c r="M28" t="inlineStr"/>
-      <c r="N28" t="inlineStr"/>
-      <c r="O28" t="inlineStr"/>
-      <c r="P28" t="inlineStr"/>
-      <c r="Q28" t="inlineStr"/>
-      <c r="R28" t="inlineStr"/>
+          <t>0440140449</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>121 Exhibition Street, Melbourne VIC 3000</t>
+        </is>
+      </c>
+      <c r="N28" t="n">
+        <v>5</v>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>Plumbing, Gas</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>#EA4335</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2283,12 +2279,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>charles_jackson</t>
+          <t>isabella_lopez</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>charles.jackson@example.com</t>
+          <t>isabella.lopez@example.com</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2298,40 +2294,40 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>0443035038</t>
+          <t>0455268745</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>623 Dohertys Road, Tarneit VIC 3029</t>
+          <t>392 Rathdowne Street, Carlton VIC 3053</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2025-10-30 12:00</t>
+          <t>2025-11-01 16:00</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>2025-10-30 15:00</t>
+          <t>2025-11-01 18:00</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Plumbing</t>
+          <t>HVAC</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Emergency Callout</t>
+          <t>HVAC Maintenance</t>
         </is>
       </c>
       <c r="M29" t="inlineStr"/>
@@ -2344,17 +2340,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Customer</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>amelia_moore</t>
+          <t>tech_riley</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>amelia.moore@example.com</t>
+          <t>tech.riley@company.com</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2364,48 +2360,44 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>0497918537</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>350 Mulgrave Business Park, Mulgrave VIC 3170</t>
-        </is>
-      </c>
-      <c r="G30" t="n">
-        <v>60</v>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>2025-11-01 11:00</t>
-        </is>
-      </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>2025-11-01 15:00</t>
-        </is>
-      </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>Gas</t>
-        </is>
-      </c>
-      <c r="K30" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="L30" t="inlineStr">
-        <is>
-          <t>Gas Leak Repair</t>
-        </is>
-      </c>
-      <c r="M30" t="inlineStr"/>
-      <c r="N30" t="inlineStr"/>
-      <c r="O30" t="inlineStr"/>
-      <c r="P30" t="inlineStr"/>
-      <c r="Q30" t="inlineStr"/>
-      <c r="R30" t="inlineStr"/>
+          <t>0413343175</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="inlineStr"/>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>782 Bridge Road, Richmond VIC 3121</t>
+        </is>
+      </c>
+      <c r="N30" t="n">
+        <v>6</v>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>Electric, HVAC, IT</t>
+        </is>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>#34A853</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2415,12 +2407,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>avery_allen</t>
+          <t>abigail_harris</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>avery.allen@example.com</t>
+          <t>abigail.harris@example.com</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2430,30 +2422,30 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>0472267893</t>
+          <t>0483030063</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>991 Lygon Street, Carlton VIC 3053</t>
+          <t>175 Lygon Street, Carlton VIC 3053</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2025-10-31 13:00</t>
+          <t>2025-11-01 12:00</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>2025-10-31 16:00</t>
+          <t>2025-11-01 14:00</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>HVAC</t>
+          <t>Plumbing</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -2463,7 +2455,7 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>HVAC Maintenance</t>
+          <t>Emergency Callout</t>
         </is>
       </c>
       <c r="M31" t="inlineStr"/>
@@ -2476,17 +2468,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Customer</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>tech_cameron</t>
+          <t>matthew_sanchez</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>tech.cameron@company.com</t>
+          <t>matthew.sanchez@example.com</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -2496,59 +2488,63 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>0461976438</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr"/>
-      <c r="H32" t="inlineStr"/>
-      <c r="I32" t="inlineStr"/>
-      <c r="J32" t="inlineStr"/>
-      <c r="K32" t="inlineStr"/>
-      <c r="L32" t="inlineStr"/>
-      <c r="M32" t="inlineStr">
-        <is>
-          <t>570 Ferntree Gully Road, Mulgrave VIC 3170</t>
-        </is>
-      </c>
-      <c r="N32" t="n">
-        <v>8</v>
-      </c>
-      <c r="O32" t="inlineStr">
-        <is>
-          <t>09:00</t>
-        </is>
-      </c>
-      <c r="P32" t="inlineStr">
-        <is>
-          <t>18:00</t>
-        </is>
-      </c>
-      <c r="Q32" t="inlineStr">
-        <is>
-          <t>Plumbing, Gas, Carpentry</t>
-        </is>
-      </c>
-      <c r="R32" t="inlineStr">
-        <is>
-          <t>#FF6D01</t>
-        </is>
-      </c>
+          <t>0477882487</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>443 Nicholson Street, Footscray VIC 3011</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
+        <v>120</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2025-11-01 13:00</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>2025-11-01 14:00</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Security</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>Safety Inspection</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr"/>
+      <c r="N32" t="inlineStr"/>
+      <c r="O32" t="inlineStr"/>
+      <c r="P32" t="inlineStr"/>
+      <c r="Q32" t="inlineStr"/>
+      <c r="R32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Customer</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>elizabeth_lewis</t>
+          <t>tech_avery</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>elizabeth.lewis@example.com</t>
+          <t>tech.avery@company.com</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -2558,63 +2554,59 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>0415544979</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>778 Chapel Street, South Yarra VIC 3141</t>
-        </is>
-      </c>
-      <c r="G33" t="n">
-        <v>120</v>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>2025-11-05 13:00</t>
-        </is>
-      </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>2025-11-05 15:00</t>
-        </is>
-      </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>Plumbing</t>
-        </is>
-      </c>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="L33" t="inlineStr">
-        <is>
-          <t>Plumbing Issue</t>
-        </is>
-      </c>
-      <c r="M33" t="inlineStr"/>
-      <c r="N33" t="inlineStr"/>
-      <c r="O33" t="inlineStr"/>
-      <c r="P33" t="inlineStr"/>
-      <c r="Q33" t="inlineStr"/>
-      <c r="R33" t="inlineStr"/>
+          <t>0437287719</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="inlineStr"/>
+      <c r="J33" t="inlineStr"/>
+      <c r="K33" t="inlineStr"/>
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>327 Acland Street, St Kilda VIC 3182</t>
+        </is>
+      </c>
+      <c r="N33" t="n">
+        <v>5</v>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>Roofing, Carpentry, Cleaning</t>
+        </is>
+      </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>#EA4335</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Customer</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>olivia_davis</t>
+          <t>tech_blake</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>olivia.davis@example.com</t>
+          <t>tech.blake@company.com</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2624,48 +2616,44 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>0480238744</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>871 Collins Street, Melbourne VIC 3000</t>
-        </is>
-      </c>
-      <c r="G34" t="n">
-        <v>180</v>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>2025-11-05 12:00</t>
-        </is>
-      </c>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>2025-11-05 14:00</t>
-        </is>
-      </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>Plumbing</t>
-        </is>
-      </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="L34" t="inlineStr">
-        <is>
-          <t>Routine Service</t>
-        </is>
-      </c>
-      <c r="M34" t="inlineStr"/>
-      <c r="N34" t="inlineStr"/>
-      <c r="O34" t="inlineStr"/>
-      <c r="P34" t="inlineStr"/>
-      <c r="Q34" t="inlineStr"/>
-      <c r="R34" t="inlineStr"/>
+          <t>0462342161</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr"/>
+      <c r="J34" t="inlineStr"/>
+      <c r="K34" t="inlineStr"/>
+      <c r="L34" t="inlineStr"/>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>824 Central Road, Clayton VIC 3168</t>
+        </is>
+      </c>
+      <c r="N34" t="n">
+        <v>5</v>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>Plumbing, Cleaning</t>
+        </is>
+      </c>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>#FBBC05</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2675,12 +2663,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>mark_robinson</t>
+          <t>avery_allen</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>mark.robinson@example.com</t>
+          <t>avery.allen@example.com</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -2690,40 +2678,40 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>0461038784</t>
+          <t>0467264138</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>354 Derrimut Road, Tarneit VIC 3029</t>
+          <t>605 Dohertys Road, Tarneit VIC 3029</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2025-11-03 12:00</t>
+          <t>2025-11-01 08:00</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>2025-11-03 14:00</t>
+          <t>2025-11-01 10:00</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Plumbing</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>System Upgrade</t>
+          <t>Plumbing Issue</t>
         </is>
       </c>
       <c r="M35" t="inlineStr"/>
@@ -2741,12 +2729,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>joseph_anderson</t>
+          <t>thomas_taylor</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>joseph.anderson@example.com</t>
+          <t>thomas.taylor@example.com</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -2756,12 +2744,12 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>0498717231</t>
+          <t>0416270241</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>266 Lygon Street, Carlton VIC 3053</t>
+          <t>170 Flinders Street, Melbourne VIC 3000</t>
         </is>
       </c>
       <c r="G36" t="n">
@@ -2769,27 +2757,27 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2025-11-01 10:00</t>
+          <t>2025-11-01 15:00</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>2025-11-01 12:00</t>
+          <t>2025-11-01 16:00</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>IT</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Gas Leak Repair</t>
+          <t>System Upgrade</t>
         </is>
       </c>
       <c r="M36" t="inlineStr"/>
@@ -2802,17 +2790,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Customer</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>tech_morgan</t>
+          <t>evelyn_thompson</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>tech.morgan@company.com</t>
+          <t>evelyn.thompson@example.com</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -2822,59 +2810,63 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>0415960373</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr"/>
-      <c r="G37" t="inlineStr"/>
-      <c r="H37" t="inlineStr"/>
-      <c r="I37" t="inlineStr"/>
-      <c r="J37" t="inlineStr"/>
-      <c r="K37" t="inlineStr"/>
-      <c r="L37" t="inlineStr"/>
-      <c r="M37" t="inlineStr">
-        <is>
-          <t>906 Swanston Street, Melbourne VIC 3000</t>
-        </is>
-      </c>
-      <c r="N37" t="n">
-        <v>8</v>
-      </c>
-      <c r="O37" t="inlineStr">
-        <is>
-          <t>08:00</t>
-        </is>
-      </c>
-      <c r="P37" t="inlineStr">
-        <is>
-          <t>18:00</t>
-        </is>
-      </c>
-      <c r="Q37" t="inlineStr">
-        <is>
-          <t>Gas, HVAC, Plumbing</t>
-        </is>
-      </c>
-      <c r="R37" t="inlineStr">
-        <is>
-          <t>#34A853</t>
-        </is>
-      </c>
+          <t>0484495620</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>842 Nicholson Street, Footscray VIC 3011</t>
+        </is>
+      </c>
+      <c r="G37" t="n">
+        <v>180</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2025-11-01 11:00</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>2025-11-01 13:00</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>Gas</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>Gas Leak Repair</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr"/>
+      <c r="N37" t="inlineStr"/>
+      <c r="O37" t="inlineStr"/>
+      <c r="P37" t="inlineStr"/>
+      <c r="Q37" t="inlineStr"/>
+      <c r="R37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Customer</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>tech_jamie</t>
+          <t>paul_scott</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>tech.jamie@company.com</t>
+          <t>paul.scott@example.com</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -2884,44 +2876,48 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>0424240619</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr"/>
-      <c r="G38" t="inlineStr"/>
-      <c r="H38" t="inlineStr"/>
-      <c r="I38" t="inlineStr"/>
-      <c r="J38" t="inlineStr"/>
-      <c r="K38" t="inlineStr"/>
-      <c r="L38" t="inlineStr"/>
-      <c r="M38" t="inlineStr">
-        <is>
-          <t>49 Swan Street, Richmond VIC 3121</t>
-        </is>
-      </c>
-      <c r="N38" t="n">
-        <v>8</v>
-      </c>
-      <c r="O38" t="inlineStr">
-        <is>
-          <t>08:00</t>
-        </is>
-      </c>
-      <c r="P38" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
-      <c r="Q38" t="inlineStr">
-        <is>
-          <t>Electric, Plumbing, Security</t>
-        </is>
-      </c>
-      <c r="R38" t="inlineStr">
-        <is>
-          <t>#4285F4</t>
-        </is>
-      </c>
+          <t>0429580246</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>595 Central Road, Clayton VIC 3168</t>
+        </is>
+      </c>
+      <c r="G38" t="n">
+        <v>120</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2025-11-01 16:00</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>2025-11-01 18:00</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>Gas</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>Gas Leak Repair</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr"/>
+      <c r="N38" t="inlineStr"/>
+      <c r="O38" t="inlineStr"/>
+      <c r="P38" t="inlineStr"/>
+      <c r="Q38" t="inlineStr"/>
+      <c r="R38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2931,12 +2927,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>isabella_lopez</t>
+          <t>emma_garcia</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>isabella.lopez@example.com</t>
+          <t>emma.garcia@example.com</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -2946,30 +2942,30 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>0434109521</t>
+          <t>0453519669</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>30 Flinders Street, Melbourne VIC 3000</t>
+          <t>903 Springvale Road, Mulgrave VIC 3170</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2025-11-01 10:00</t>
+          <t>2025-11-01 09:00</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>2025-11-01 13:00</t>
+          <t>2025-11-01 11:00</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Plumbing</t>
+          <t>IT</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -2979,7 +2975,7 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Routine Service</t>
+          <t>System Upgrade</t>
         </is>
       </c>
       <c r="M39" t="inlineStr"/>
@@ -2997,12 +2993,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>emily_clark</t>
+          <t>mary_johnson</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>emily.clark@example.com</t>
+          <t>mary.johnson@example.com</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -3012,40 +3008,40 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>0492982933</t>
+          <t>0426130572</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>195 Bridge Road, Richmond VIC 3121</t>
+          <t>18 Acland Street, St Kilda VIC 3182</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2025-11-02 10:00</t>
+          <t>2025-11-01 16:00</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>2025-11-02 14:00</t>
+          <t>2025-11-01 18:00</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Plumbing</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Emergency Callout</t>
+          <t>Gas Leak Repair</t>
         </is>
       </c>
       <c r="M40" t="inlineStr"/>
@@ -3063,12 +3059,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>tech_drew</t>
+          <t>tech_dakota</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>tech.drew@company.com</t>
+          <t>tech.dakota@company.com</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -3078,7 +3074,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>0435373250</t>
+          <t>0428587579</t>
         </is>
       </c>
       <c r="F41" t="inlineStr"/>
@@ -3090,30 +3086,30 @@
       <c r="L41" t="inlineStr"/>
       <c r="M41" t="inlineStr">
         <is>
-          <t>854 Ferntree Gully Road, Mulgrave VIC 3170</t>
+          <t>183 Bridge Road, Richmond VIC 3121</t>
         </is>
       </c>
       <c r="N41" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>IT, Electric</t>
+          <t>HVAC, Plumbing</t>
         </is>
       </c>
       <c r="R41" t="inlineStr">
         <is>
-          <t>#4285F4</t>
+          <t>#FBBC05</t>
         </is>
       </c>
     </row>
@@ -3125,12 +3121,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>william_hernandez</t>
+          <t>harper_martin</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>william.hernandez@example.com</t>
+          <t>harper.martin@example.com</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -3140,30 +3136,30 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>0495663133</t>
+          <t>0490505977</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>450 Dandenong Railway Station, Dandenong VIC 3175</t>
+          <t>865 Chapel Street, South Yarra VIC 3141</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2025-11-02 14:00</t>
+          <t>2025-11-01 08:00</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>2025-11-02 17:00</t>
+          <t>2025-11-01 10:00</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Plumbing</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
@@ -3173,7 +3169,7 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Gas Leak Repair</t>
+          <t>Emergency Callout</t>
         </is>
       </c>
       <c r="M42" t="inlineStr"/>
@@ -3191,12 +3187,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>john_smith</t>
+          <t>donald_young</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>john.smith@example.com</t>
+          <t>donald.young@example.com</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -3206,30 +3202,30 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>0440468624</t>
+          <t>0446466682</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>859 Springvale Road, Mulgrave VIC 3170</t>
+          <t>106 Nicholson Street, Footscray VIC 3011</t>
         </is>
       </c>
       <c r="G43" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>2025-10-30 14:00</t>
+          <t>2025-11-01 16:00</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>2025-10-30 17:00</t>
+          <t>2025-11-01 18:00</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Electric</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
@@ -3239,7 +3235,7 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Gas Leak Repair</t>
+          <t>Appliance Installation</t>
         </is>
       </c>
       <c r="M43" t="inlineStr"/>
@@ -3272,7 +3268,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>0481874380</t>
+          <t>0484389248</t>
         </is>
       </c>
       <c r="F44" t="inlineStr"/>
@@ -3284,20 +3280,20 @@
       <c r="L44" t="inlineStr"/>
       <c r="M44" t="inlineStr">
         <is>
-          <t>941 Clayton Campus, Monash University, Clayton VIC 3168</t>
+          <t>805 Commercial Road, South Yarra VIC 3141</t>
         </is>
       </c>
       <c r="N44" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="Q44" t="inlineStr">
@@ -3307,7 +3303,7 @@
       </c>
       <c r="R44" t="inlineStr">
         <is>
-          <t>#34A853</t>
+          <t>#FBBC05</t>
         </is>
       </c>
     </row>
@@ -3319,12 +3315,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>charlotte_thomas</t>
+          <t>daniel_white</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>charlotte.thomas@example.com</t>
+          <t>daniel.white@example.com</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3334,25 +3330,25 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>0466394905</t>
+          <t>0476768071</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>718 Derrimut Road, Tarneit VIC 3029</t>
+          <t>637 Rathdowne Street, Carlton VIC 3053</t>
         </is>
       </c>
       <c r="G45" t="n">
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>2025-11-02 09:00</t>
+          <t>2025-11-01 08:00</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>2025-11-02 11:00</t>
+          <t>2025-11-01 09:00</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
@@ -3367,7 +3363,7 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Maintenance Check</t>
+          <t>Electrical Fault</t>
         </is>
       </c>
       <c r="M45" t="inlineStr"/>
@@ -3385,12 +3381,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>matthew_sanchez</t>
+          <t>olivia_davis</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>matthew.sanchez@example.com</t>
+          <t>olivia.davis@example.com</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3400,30 +3396,30 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>0473914138</t>
+          <t>0433737847</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>664 Collins Street, Melbourne VIC 3000</t>
+          <t>957 Clayton Campus, Monash University, Clayton VIC 3168</t>
         </is>
       </c>
       <c r="G46" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2025-11-02 10:00</t>
+          <t>2025-11-01 10:00</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>2025-11-02 12:00</t>
+          <t>2025-11-01 11:00</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Plumbing</t>
+          <t>Electric</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
@@ -3433,7 +3429,7 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Routine Service</t>
+          <t>Maintenance Check</t>
         </is>
       </c>
       <c r="M46" t="inlineStr"/>
@@ -3451,12 +3447,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>richard_gonzalez</t>
+          <t>william_hernandez</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>richard.gonzalez@example.com</t>
+          <t>william.hernandez@example.com</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -3466,30 +3462,30 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>0470315804</t>
+          <t>0442165391</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>534 Swan Street, Richmond VIC 3121</t>
+          <t>682 Clayton Road, Clayton VIC 3168</t>
         </is>
       </c>
       <c r="G47" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>2025-11-03 12:00</t>
+          <t>2025-11-01 15:00</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>2025-11-03 16:00</t>
+          <t>2025-11-01 16:00</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Electric</t>
+          <t>Plumbing</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -3499,7 +3495,7 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Electrical Fault</t>
+          <t>Plumbing Issue</t>
         </is>
       </c>
       <c r="M47" t="inlineStr"/>
@@ -3517,12 +3513,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>james_miller</t>
+          <t>david_williams</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>james.miller@example.com</t>
+          <t>david.williams@example.com</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -3532,25 +3528,25 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>0453896230</t>
+          <t>0427779725</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>561 Bridge Road, Richmond VIC 3121</t>
+          <t>552 Dandenong Railway Station, Dandenong VIC 3175</t>
         </is>
       </c>
       <c r="G48" t="n">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>2025-10-30 13:00</t>
+          <t>2025-11-01 09:00</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>2025-10-30 15:00</t>
+          <t>2025-11-01 11:00</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
@@ -3560,12 +3556,12 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Appliance Installation</t>
+          <t>Maintenance Check</t>
         </is>
       </c>
       <c r="M48" t="inlineStr"/>
@@ -3583,12 +3579,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>tech_riley</t>
+          <t>tech_drew</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>tech.riley@company.com</t>
+          <t>tech.drew@company.com</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -3598,7 +3594,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>0436692676</t>
+          <t>0428989390</t>
         </is>
       </c>
       <c r="F49" t="inlineStr"/>
@@ -3610,25 +3606,25 @@
       <c r="L49" t="inlineStr"/>
       <c r="M49" t="inlineStr">
         <is>
-          <t>427 Swan Street, Richmond VIC 3121</t>
+          <t>531 Ferntree Gully Road, Mulgrave VIC 3170</t>
         </is>
       </c>
       <c r="N49" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="Q49" t="inlineStr">
         <is>
-          <t>Electric, HVAC, IT</t>
+          <t>IT, Electric</t>
         </is>
       </c>
       <c r="R49" t="inlineStr">
@@ -3640,17 +3636,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Customer</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>tech_jordan</t>
+          <t>sophia_martinez</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>tech.jordan@company.com</t>
+          <t>sophia.martinez@example.com</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -3660,44 +3656,48 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>0467399092</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr"/>
-      <c r="G50" t="inlineStr"/>
-      <c r="H50" t="inlineStr"/>
-      <c r="I50" t="inlineStr"/>
-      <c r="J50" t="inlineStr"/>
-      <c r="K50" t="inlineStr"/>
-      <c r="L50" t="inlineStr"/>
-      <c r="M50" t="inlineStr">
-        <is>
-          <t>38 Robinson Street, Dandenong VIC 3175</t>
-        </is>
-      </c>
-      <c r="N50" t="n">
-        <v>8</v>
-      </c>
-      <c r="O50" t="inlineStr">
-        <is>
-          <t>08:00</t>
-        </is>
-      </c>
-      <c r="P50" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
-      <c r="Q50" t="inlineStr">
-        <is>
-          <t>Electric, Solar</t>
-        </is>
-      </c>
-      <c r="R50" t="inlineStr">
-        <is>
-          <t>#4285F4</t>
-        </is>
-      </c>
+          <t>0476632499</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>484 Elizabeth Street, Melbourne VIC 3000</t>
+        </is>
+      </c>
+      <c r="G50" t="n">
+        <v>120</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2025-11-01 16:00</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>2025-11-01 18:00</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>Electric</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>Maintenance Check</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr"/>
+      <c r="N50" t="inlineStr"/>
+      <c r="O50" t="inlineStr"/>
+      <c r="P50" t="inlineStr"/>
+      <c r="Q50" t="inlineStr"/>
+      <c r="R50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -3707,12 +3707,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>emma_garcia</t>
+          <t>michael_jones</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>emma.garcia@example.com</t>
+          <t>michael.jones@example.com</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -3722,12 +3722,12 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>0489581058</t>
+          <t>0475007409</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>369 Commercial Road, South Yarra VIC 3141</t>
+          <t>986 Ferntree Gully Road, Mulgrave VIC 3170</t>
         </is>
       </c>
       <c r="G51" t="n">
@@ -3735,17 +3735,17 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>2025-11-04 11:00</t>
+          <t>2025-11-01 11:00</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>2025-11-04 13:00</t>
+          <t>2025-11-01 12:00</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Electric</t>
+          <t>Plumbing</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -3755,7 +3755,7 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Appliance Installation</t>
+          <t>Plumbing Issue</t>
         </is>
       </c>
       <c r="M51" t="inlineStr"/>

</xml_diff>

<commit_message>
Add address autocomplete to edit multiple form and fix formset management form issues
</commit_message>
<xml_diff>
--- a/sample_data_50_people.xlsx
+++ b/sample_data_50_people.xlsx
@@ -533,12 +533,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>tech_morgan</t>
+          <t>tech_riley</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>tech.morgan@company.com</t>
+          <t>tech.riley@company.com</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -548,7 +548,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0462965398</t>
+          <t>0410782057</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
@@ -560,47 +560,47 @@
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
-          <t>63 Rathdowne Street, Carlton VIC 3053</t>
+          <t>922 Collins Street, Melbourne VIC 3000</t>
         </is>
       </c>
       <c r="N2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>06:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Gas, HVAC, Plumbing</t>
+          <t>Behaviour Support, Therapy Access, Assistive Tech</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>#FBBC05</t>
+          <t>#EA4335</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Customer</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>emily_clark</t>
+          <t>tech_jordan</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>emily.clark@example.com</t>
+          <t>tech.jordan@company.com</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -610,63 +610,59 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0456011717</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>944 Nicholson Street, Footscray VIC 3011</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>90</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>2025-11-01 10:00</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>2025-11-01 12:00</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Electric</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>Appliance Installation</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr"/>
+          <t>0439651693</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>699 Bridge Road, Richmond VIC 3121</t>
+        </is>
+      </c>
+      <c r="N3" t="n">
+        <v>4</v>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Transport, Community Access</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>#34A853</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Customer</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>tech_jamie</t>
+          <t>daniel_white</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>tech.jamie@company.com</t>
+          <t>daniel.white@example.com</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -676,59 +672,63 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0481895582</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>706 Nicholson Street, Footscray VIC 3011</t>
-        </is>
-      </c>
-      <c r="N4" t="n">
-        <v>6</v>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>11:00</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>Electric, Plumbing, Security</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>#4285F4</t>
-        </is>
-      </c>
+          <t>0447050073</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>456 Bourke Street, Melbourne VIC 3000</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>180</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2025-11-01 12:00</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>2025-11-01 14:00</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Therapy Access</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Therapy Access</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Customer</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>tech_cameron</t>
+          <t>elizabeth_lewis</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>tech.cameron@company.com</t>
+          <t>elizabeth.lewis@example.com</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -738,44 +738,48 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0496250839</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>255 Springvale Road, Mulgrave VIC 3170</t>
-        </is>
-      </c>
-      <c r="N5" t="n">
-        <v>8</v>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>06:00</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>14:00</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>Plumbing, Gas, Carpentry</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>#EA4335</t>
-        </is>
-      </c>
+          <t>0496168775</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>55 Clayton Road, Clayton VIC 3168</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>180</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2025-11-01 13:00</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2025-11-01 15:00</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Therapy Access</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Therapy Access</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -785,12 +789,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>mark_robinson</t>
+          <t>victoria_wright</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>mark.robinson@example.com</t>
+          <t>victoria.wright@example.com</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -800,40 +804,40 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0439676172</t>
+          <t>0477185539</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>147 Swan Street, Richmond VIC 3121</t>
+          <t>88 Dandenong Road, Dandenong VIC 3175</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
+          <t>2025-11-01 12:00</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
           <t>2025-11-01 14:00</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>2025-11-01 16:00</t>
-        </is>
-      </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Support Coordination</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>System Upgrade</t>
+          <t>Support Coordination</t>
         </is>
       </c>
       <c r="M6" t="inlineStr"/>
@@ -846,17 +850,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Customer</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>tech_sage</t>
+          <t>charlotte_thomas</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>tech.sage@company.com</t>
+          <t>charlotte.thomas@example.com</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -866,44 +870,48 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0486252294</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>968 Rathdowne Street, Carlton VIC 3053</t>
-        </is>
-      </c>
-      <c r="N7" t="n">
-        <v>5</v>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>13:00</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>18:00</t>
-        </is>
-      </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>IT, Security</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>#EA4335</t>
-        </is>
-      </c>
+          <t>0415838888</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>123 Collins Street, Melbourne VIC 3000</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>180</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2025-11-01 13:00</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>2025-11-01 15:00</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Support Coordination</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Support Coordination</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -913,12 +921,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>sarah_brown</t>
+          <t>emily_clark</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>sarah.brown@example.com</t>
+          <t>emily.clark@example.com</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -928,40 +936,40 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0462705300</t>
+          <t>0487022188</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>800 Ferntree Gully Road, Mulgrave VIC 3170</t>
+          <t>789 Swanston Street, Melbourne VIC 3000</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-11-01 14:00</t>
+          <t>2025-11-01 16:00</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>2025-11-01 15:00</t>
+          <t>2025-11-01 17:00</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Assistive Tech</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>System Upgrade</t>
+          <t>Assistive Tech</t>
         </is>
       </c>
       <c r="M8" t="inlineStr"/>
@@ -979,12 +987,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>charlotte_thomas</t>
+          <t>anthony_ramirez</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>charlotte.thomas@example.com</t>
+          <t>anthony.ramirez@example.com</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -994,40 +1002,40 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0440744539</t>
+          <t>0428391621</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>940 Commercial Road, South Yarra VIC 3141</t>
+          <t>789 Swanston Street, Melbourne VIC 3000</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-11-01 10:00</t>
+          <t>2025-11-01 11:00</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>2025-11-01 11:00</t>
+          <t>2025-11-01 13:00</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Plumbing</t>
+          <t>Support Coordination</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Emergency Callout</t>
+          <t>Support Coordination</t>
         </is>
       </c>
       <c r="M9" t="inlineStr"/>
@@ -1045,12 +1053,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>tech_reese</t>
+          <t>tech_casey</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>tech.reese@company.com</t>
+          <t>tech.casey@company.com</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1060,7 +1068,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0462996689</t>
+          <t>0414715939</t>
         </is>
       </c>
       <c r="F10" t="inlineStr"/>
@@ -1072,30 +1080,30 @@
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr">
         <is>
-          <t>364 Derrimut Road, Tarneit VIC 3029</t>
+          <t>637 Commercial Road, South Yarra VIC 3141</t>
         </is>
       </c>
       <c r="N10" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>06:00</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Electric, Solar, HVAC, IT</t>
+          <t>Behaviour Support, Therapy Access</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>#FBBC05</t>
+          <t>#EA4335</t>
         </is>
       </c>
     </row>
@@ -1107,12 +1115,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>tech_quinn</t>
+          <t>tech_taylor</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>tech.quinn@company.com</t>
+          <t>tech.taylor@company.com</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1122,7 +1130,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0494373117</t>
+          <t>0439710693</t>
         </is>
       </c>
       <c r="F11" t="inlineStr"/>
@@ -1134,30 +1142,30 @@
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr">
         <is>
-          <t>709 Dandenong Railway Station, Dandenong VIC 3175</t>
+          <t>135 Fitzroy Street, St Kilda VIC 3182</t>
         </is>
       </c>
       <c r="N11" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Roofing, Carpentry</t>
+          <t>Transport, Community Access, Therapy Access</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>#FF6D01</t>
+          <t>#FBBC05</t>
         </is>
       </c>
     </row>
@@ -1169,12 +1177,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>elizabeth_lewis</t>
+          <t>matthew_sanchez</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>elizabeth.lewis@example.com</t>
+          <t>matthew.sanchez@example.com</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1184,30 +1192,30 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>0480601698</t>
+          <t>0478366784</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>243 Fitzroy Street, St Kilda VIC 3182</t>
+          <t>789 Swanston Street, Melbourne VIC 3000</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-11-01 15:00</t>
+          <t>2025-11-01 09:00</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>2025-11-01 17:00</t>
+          <t>2025-11-01 10:00</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Plumbing</t>
+          <t>Life Skills Training</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1217,7 +1225,7 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Routine Service</t>
+          <t>Life Skills Training</t>
         </is>
       </c>
       <c r="M12" t="inlineStr"/>
@@ -1230,17 +1238,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Customer</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>tech_jordan</t>
+          <t>michael_jones</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>tech.jordan@company.com</t>
+          <t>michael.jones@example.com</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1250,59 +1258,63 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>0474801753</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>433 Lygon Street, Carlton VIC 3053</t>
-        </is>
-      </c>
-      <c r="N13" t="n">
-        <v>5</v>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>06:00</t>
-        </is>
-      </c>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t>11:00</t>
-        </is>
-      </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>Electric, Solar</t>
-        </is>
-      </c>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>#FF6D01</t>
-        </is>
-      </c>
+          <t>0445309925</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>92 Exhibition Street, Melbourne VIC 3000</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>180</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2025-11-01 13:00</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>2025-11-01 14:00</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Life Skills Training</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Life Skills Training</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr"/>
+      <c r="R13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Customer</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>christopher_lee</t>
+          <t>tech_alex</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>christopher.lee@example.com</t>
+          <t>tech.alex@company.com</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1312,48 +1324,44 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>0472824095</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>89 Derrimut Road, Tarneit VIC 3029</t>
-        </is>
-      </c>
-      <c r="G14" t="n">
-        <v>180</v>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>2025-11-01 12:00</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>2025-11-01 14:00</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>Gas</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>Gas Leak Repair</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="inlineStr"/>
+          <t>0473115146</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>837 Clayton Road, Clayton VIC 3168</t>
+        </is>
+      </c>
+      <c r="N14" t="n">
+        <v>5</v>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>Personal care, Domestic Assistance</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>#4285F4</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1363,12 +1371,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>robert_rodriguez</t>
+          <t>harper_martin</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>robert.rodriguez@example.com</t>
+          <t>harper.martin@example.com</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1378,30 +1386,30 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>0468358757</t>
+          <t>0417414568</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>461 Bridge Road, Richmond VIC 3121</t>
+          <t>456 Bourke Street, Melbourne VIC 3000</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-11-01 13:00</t>
+          <t>2025-11-01 10:00</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>2025-11-01 15:00</t>
+          <t>2025-11-01 12:00</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Electric</t>
+          <t>Domestic Assistance</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1411,7 +1419,7 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Electrical Fault</t>
+          <t>Domestic Assistance</t>
         </is>
       </c>
       <c r="M15" t="inlineStr"/>
@@ -1429,12 +1437,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>mia_wilson</t>
+          <t>thomas_taylor</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>mia.wilson@example.com</t>
+          <t>thomas.taylor@example.com</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1444,16 +1452,16 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>0476672201</t>
+          <t>0474234121</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>317 Springvale Road, Mulgrave VIC 3170</t>
+          <t>123 Collins Street, Melbourne VIC 3000</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -1467,7 +1475,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Plumbing</t>
+          <t>Therapy Access</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1477,7 +1485,7 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Routine Service</t>
+          <t>Therapy Access</t>
         </is>
       </c>
       <c r="M16" t="inlineStr"/>
@@ -1495,12 +1503,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>amelia_moore</t>
+          <t>john_smith</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>amelia.moore@example.com</t>
+          <t>john.smith@example.com</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1510,16 +1518,16 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0497692482</t>
+          <t>0465138213</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>86 Clayton Campus, Monash University, Clayton VIC 3168</t>
+          <t>145 Fitzroy Street, St Kilda VIC 3182</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -1528,22 +1536,22 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>2025-11-01 18:00</t>
+          <t>2025-11-01 17:00</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Plumbing</t>
+          <t>Life Skills Training</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>High</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Emergency Callout</t>
+          <t>Life Skills Training</t>
         </is>
       </c>
       <c r="M17" t="inlineStr"/>
@@ -1561,12 +1569,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>charles_jackson</t>
+          <t>sofia_walker</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>charles.jackson@example.com</t>
+          <t>sofia.walker@example.com</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1576,30 +1584,30 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0493596754</t>
+          <t>0480697736</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>975 Chapel Street, South Yarra VIC 3141</t>
+          <t>55 Clayton Road, Clayton VIC 3168</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-11-01 08:00</t>
+          <t>2025-11-01 16:00</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>2025-11-01 10:00</t>
+          <t>2025-11-01 18:00</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Security</t>
+          <t>Personal care</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1609,7 +1617,7 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Safety Inspection</t>
+          <t>Personal care</t>
         </is>
       </c>
       <c r="M18" t="inlineStr"/>
@@ -1622,17 +1630,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Customer</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>sofia_walker</t>
+          <t>tech_reese</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>sofia.walker@example.com</t>
+          <t>tech.reese@company.com</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1642,48 +1650,44 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0465228749</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>846 Bridge Road, Richmond VIC 3121</t>
-        </is>
-      </c>
-      <c r="G19" t="n">
-        <v>90</v>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>2025-11-01 13:00</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>2025-11-01 14:00</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>Plumbing</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>Plumbing Issue</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr"/>
-      <c r="N19" t="inlineStr"/>
-      <c r="O19" t="inlineStr"/>
-      <c r="P19" t="inlineStr"/>
-      <c r="Q19" t="inlineStr"/>
-      <c r="R19" t="inlineStr"/>
+          <t>0425366081</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>615 Derrimut Road, Tarneit VIC 3029</t>
+        </is>
+      </c>
+      <c r="N19" t="n">
+        <v>5</v>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>Transport, Community Access, Therapy Access, Life Skills Training</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>#34A853</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1693,12 +1697,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>anthony_ramirez</t>
+          <t>david_williams</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>anthony.ramirez@example.com</t>
+          <t>david.williams@example.com</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1708,16 +1712,16 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>0446985387</t>
+          <t>0422894853</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>813 Dandenong Railway Station, Dandenong VIC 3175</t>
+          <t>43 Commercial Road, South Yarra VIC 3141</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
@@ -1731,17 +1735,17 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Domestic Assistance</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>System Upgrade</t>
+          <t>Domestic Assistance</t>
         </is>
       </c>
       <c r="M20" t="inlineStr"/>
@@ -1759,12 +1763,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>john_smith</t>
+          <t>mary_johnson</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>john.smith@example.com</t>
+          <t>mary.johnson@example.com</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1774,30 +1778,30 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>0412924588</t>
+          <t>0437514338</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>587 Dohertys Road, Tarneit VIC 3029</t>
+          <t>230 Nicholson Street, Footscray VIC 3011</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2025-11-01 13:00</t>
+          <t>2025-11-01 09:00</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>2025-11-01 14:00</t>
+          <t>2025-11-01 10:00</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Electric</t>
+          <t>Transport</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -1807,7 +1811,7 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Electrical Fault</t>
+          <t>Transport</t>
         </is>
       </c>
       <c r="M21" t="inlineStr"/>
@@ -1825,12 +1829,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>steven_king</t>
+          <t>mark_robinson</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>steven.king@example.com</t>
+          <t>mark.robinson@example.com</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1840,12 +1844,12 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>0444593646</t>
+          <t>0493688501</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>16 Fitzroy Street, St Kilda VIC 3182</t>
+          <t>55 Clayton Road, Clayton VIC 3168</t>
         </is>
       </c>
       <c r="G22" t="n">
@@ -1853,17 +1857,17 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2025-11-01 13:00</t>
+          <t>2025-11-01 11:00</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>2025-11-01 15:00</t>
+          <t>2025-11-01 12:00</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Therapy Access</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -1873,7 +1877,7 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Gas Leak Repair</t>
+          <t>Therapy Access</t>
         </is>
       </c>
       <c r="M22" t="inlineStr"/>
@@ -1886,17 +1890,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Customer</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>tech_casey</t>
+          <t>mia_wilson</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>tech.casey@company.com</t>
+          <t>mia.wilson@example.com</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1906,44 +1910,48 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0458791764</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
-      <c r="K23" t="inlineStr"/>
-      <c r="L23" t="inlineStr"/>
-      <c r="M23" t="inlineStr">
-        <is>
-          <t>775 Derrimut Road, Tarneit VIC 3029</t>
-        </is>
-      </c>
-      <c r="N23" t="n">
-        <v>6</v>
-      </c>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>12:00</t>
-        </is>
-      </c>
-      <c r="P23" t="inlineStr">
-        <is>
-          <t>18:00</t>
-        </is>
-      </c>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>HVAC, Electric</t>
-        </is>
-      </c>
-      <c r="R23" t="inlineStr">
-        <is>
-          <t>#FF6D01</t>
-        </is>
-      </c>
+          <t>0468158226</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>242 Nicholson Street, Footscray VIC 3011</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>90</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2025-11-01 14:00</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>2025-11-01 16:00</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Personal care</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>Personal care</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr"/>
+      <c r="R23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1953,12 +1961,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>richard_gonzalez</t>
+          <t>donald_young</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>richard.gonzalez@example.com</t>
+          <t>donald.young@example.com</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1968,12 +1976,12 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>0467607024</t>
+          <t>0464373309</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>640 Tarneit Road, Tarneit VIC 3029</t>
+          <t>55 Clayton Road, Clayton VIC 3168</t>
         </is>
       </c>
       <c r="G24" t="n">
@@ -1981,7 +1989,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2025-11-01 14:00</t>
+          <t>2025-11-01 13:00</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1991,7 +1999,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Transport</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -2001,7 +2009,7 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>System Upgrade</t>
+          <t>Transport</t>
         </is>
       </c>
       <c r="M24" t="inlineStr"/>
@@ -2019,12 +2027,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>james_miller</t>
+          <t>emma_garcia</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>james.miller@example.com</t>
+          <t>emma.garcia@example.com</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -2034,12 +2042,12 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>0493018531</t>
+          <t>0437063245</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>667 Bourke Street, Melbourne VIC 3000</t>
+          <t>511 Nicholson Street, Footscray VIC 3011</t>
         </is>
       </c>
       <c r="G25" t="n">
@@ -2047,17 +2055,17 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2025-11-01 09:00</t>
+          <t>2025-11-01 13:00</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>2025-11-01 11:00</t>
+          <t>2025-11-01 15:00</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Personal care</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2067,7 +2075,7 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Gas Leak Repair</t>
+          <t>Personal care</t>
         </is>
       </c>
       <c r="M25" t="inlineStr"/>
@@ -2085,12 +2093,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>joseph_anderson</t>
+          <t>steven_king</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>joseph.anderson@example.com</t>
+          <t>steven.king@example.com</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2100,12 +2108,12 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>0463347946</t>
+          <t>0419420614</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>806 Springvale Road, Mulgrave VIC 3170</t>
+          <t>88 Dandenong Road, Dandenong VIC 3175</t>
         </is>
       </c>
       <c r="G26" t="n">
@@ -2118,12 +2126,12 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>2025-11-01 13:00</t>
+          <t>2025-11-01 12:00</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Electric</t>
+          <t>Domestic Assistance</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2133,7 +2141,7 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Appliance Installation</t>
+          <t>Domestic Assistance</t>
         </is>
       </c>
       <c r="M26" t="inlineStr"/>
@@ -2151,12 +2159,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>victoria_wright</t>
+          <t>isabella_lopez</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>victoria.wright@example.com</t>
+          <t>isabella.lopez@example.com</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2166,40 +2174,40 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>0480182314</t>
+          <t>0412813377</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>840 Clayton Road, Clayton VIC 3168</t>
+          <t>262 Princes Highway, Dandenong VIC 3175</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
+          <t>2025-11-01 10:00</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
           <t>2025-11-01 11:00</t>
         </is>
       </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>2025-11-01 13:00</t>
-        </is>
-      </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Electric</t>
+          <t>Personal care</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Maintenance Check</t>
+          <t>Personal care</t>
         </is>
       </c>
       <c r="M27" t="inlineStr"/>
@@ -2212,17 +2220,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Customer</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>tech_alex</t>
+          <t>olivia_davis</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>tech.alex@company.com</t>
+          <t>olivia.davis@example.com</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2232,59 +2240,63 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>0440140449</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
-      <c r="I28" t="inlineStr"/>
-      <c r="J28" t="inlineStr"/>
-      <c r="K28" t="inlineStr"/>
-      <c r="L28" t="inlineStr"/>
-      <c r="M28" t="inlineStr">
-        <is>
-          <t>121 Exhibition Street, Melbourne VIC 3000</t>
-        </is>
-      </c>
-      <c r="N28" t="n">
-        <v>5</v>
-      </c>
-      <c r="O28" t="inlineStr">
-        <is>
-          <t>11:00</t>
-        </is>
-      </c>
-      <c r="P28" t="inlineStr">
-        <is>
-          <t>16:00</t>
-        </is>
-      </c>
-      <c r="Q28" t="inlineStr">
-        <is>
-          <t>Plumbing, Gas</t>
-        </is>
-      </c>
-      <c r="R28" t="inlineStr">
-        <is>
-          <t>#EA4335</t>
-        </is>
-      </c>
+          <t>0421048105</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>375 Barkly Street, Footscray VIC 3011</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
+        <v>60</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2025-11-01 16:00</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>2025-11-01 17:00</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Domestic Assistance</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>Domestic Assistance</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr"/>
+      <c r="O28" t="inlineStr"/>
+      <c r="P28" t="inlineStr"/>
+      <c r="Q28" t="inlineStr"/>
+      <c r="R28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Customer</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>isabella_lopez</t>
+          <t>tech_drew</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>isabella.lopez@example.com</t>
+          <t>tech.drew@company.com</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2294,63 +2306,59 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>0455268745</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>392 Rathdowne Street, Carlton VIC 3053</t>
-        </is>
-      </c>
-      <c r="G29" t="n">
-        <v>90</v>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>2025-11-01 16:00</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>2025-11-01 18:00</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>HVAC</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t>HVAC Maintenance</t>
-        </is>
-      </c>
-      <c r="M29" t="inlineStr"/>
-      <c r="N29" t="inlineStr"/>
-      <c r="O29" t="inlineStr"/>
-      <c r="P29" t="inlineStr"/>
-      <c r="Q29" t="inlineStr"/>
-      <c r="R29" t="inlineStr"/>
+          <t>0498162541</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>901 Mulgrave Business Park, Mulgrave VIC 3170</t>
+        </is>
+      </c>
+      <c r="N29" t="n">
+        <v>4</v>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>Support Coordination, Life Skills Training</t>
+        </is>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>#FF6D01</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Customer</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>tech_riley</t>
+          <t>christopher_lee</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>tech.riley@company.com</t>
+          <t>christopher.lee@example.com</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2360,59 +2368,63 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>0413343175</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr"/>
-      <c r="H30" t="inlineStr"/>
-      <c r="I30" t="inlineStr"/>
-      <c r="J30" t="inlineStr"/>
-      <c r="K30" t="inlineStr"/>
-      <c r="L30" t="inlineStr"/>
-      <c r="M30" t="inlineStr">
-        <is>
-          <t>782 Bridge Road, Richmond VIC 3121</t>
-        </is>
-      </c>
-      <c r="N30" t="n">
-        <v>6</v>
-      </c>
-      <c r="O30" t="inlineStr">
-        <is>
-          <t>12:00</t>
-        </is>
-      </c>
-      <c r="P30" t="inlineStr">
-        <is>
-          <t>18:00</t>
-        </is>
-      </c>
-      <c r="Q30" t="inlineStr">
-        <is>
-          <t>Electric, HVAC, IT</t>
-        </is>
-      </c>
-      <c r="R30" t="inlineStr">
-        <is>
-          <t>#34A853</t>
-        </is>
-      </c>
+          <t>0449288063</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>456 Bourke Street, Melbourne VIC 3000</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>90</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2025-11-01 13:00</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>2025-11-01 14:00</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Life Skills Training</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>Life Skills Training</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr"/>
+      <c r="N30" t="inlineStr"/>
+      <c r="O30" t="inlineStr"/>
+      <c r="P30" t="inlineStr"/>
+      <c r="Q30" t="inlineStr"/>
+      <c r="R30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Customer</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>abigail_harris</t>
+          <t>tech_jamie</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>abigail.harris@example.com</t>
+          <t>tech.jamie@company.com</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2422,63 +2434,59 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>0483030063</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>175 Lygon Street, Carlton VIC 3053</t>
-        </is>
-      </c>
-      <c r="G31" t="n">
-        <v>180</v>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>2025-11-01 12:00</t>
-        </is>
-      </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>2025-11-01 14:00</t>
-        </is>
-      </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>Plumbing</t>
-        </is>
-      </c>
-      <c r="K31" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="L31" t="inlineStr">
-        <is>
-          <t>Emergency Callout</t>
-        </is>
-      </c>
-      <c r="M31" t="inlineStr"/>
-      <c r="N31" t="inlineStr"/>
-      <c r="O31" t="inlineStr"/>
-      <c r="P31" t="inlineStr"/>
-      <c r="Q31" t="inlineStr"/>
-      <c r="R31" t="inlineStr"/>
+          <t>0443949552</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr"/>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr"/>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>648 Lygon Street, Carlton VIC 3053</t>
+        </is>
+      </c>
+      <c r="N31" t="n">
+        <v>4</v>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>Personal care, Domestic Assistance, Assistive Tech</t>
+        </is>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>#FBBC05</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Customer</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>matthew_sanchez</t>
+          <t>tech_morgan</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>matthew.sanchez@example.com</t>
+          <t>tech.morgan@company.com</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -2488,48 +2496,44 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>0477882487</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>443 Nicholson Street, Footscray VIC 3011</t>
-        </is>
-      </c>
-      <c r="G32" t="n">
-        <v>120</v>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>2025-11-01 13:00</t>
-        </is>
-      </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>2025-11-01 14:00</t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>Security</t>
-        </is>
-      </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="L32" t="inlineStr">
-        <is>
-          <t>Safety Inspection</t>
-        </is>
-      </c>
-      <c r="M32" t="inlineStr"/>
-      <c r="N32" t="inlineStr"/>
-      <c r="O32" t="inlineStr"/>
-      <c r="P32" t="inlineStr"/>
-      <c r="Q32" t="inlineStr"/>
-      <c r="R32" t="inlineStr"/>
+          <t>0457931425</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr"/>
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>449 Commercial Road, South Yarra VIC 3141</t>
+        </is>
+      </c>
+      <c r="N32" t="n">
+        <v>7</v>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>Behaviour Support, Support Coordination, Life Skills Training</t>
+        </is>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>#4285F4</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2554,7 +2558,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>0437287719</t>
+          <t>0459885132</t>
         </is>
       </c>
       <c r="F33" t="inlineStr"/>
@@ -2566,47 +2570,47 @@
       <c r="L33" t="inlineStr"/>
       <c r="M33" t="inlineStr">
         <is>
-          <t>327 Acland Street, St Kilda VIC 3182</t>
+          <t>971 Mulgrave Business Park, Mulgrave VIC 3170</t>
         </is>
       </c>
       <c r="N33" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="P33" t="inlineStr">
+        <is>
           <t>12:00</t>
         </is>
       </c>
-      <c r="P33" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>Roofing, Carpentry, Cleaning</t>
+          <t>Therapy Access, Assistive Tech</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
         <is>
-          <t>#EA4335</t>
+          <t>#4285F4</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Customer</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>tech_blake</t>
+          <t>abigail_harris</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>tech.blake@company.com</t>
+          <t>abigail.harris@example.com</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2616,44 +2620,48 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>0462342161</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr"/>
-      <c r="G34" t="inlineStr"/>
-      <c r="H34" t="inlineStr"/>
-      <c r="I34" t="inlineStr"/>
-      <c r="J34" t="inlineStr"/>
-      <c r="K34" t="inlineStr"/>
-      <c r="L34" t="inlineStr"/>
-      <c r="M34" t="inlineStr">
-        <is>
-          <t>824 Central Road, Clayton VIC 3168</t>
-        </is>
-      </c>
-      <c r="N34" t="n">
-        <v>5</v>
-      </c>
-      <c r="O34" t="inlineStr">
-        <is>
-          <t>09:00</t>
-        </is>
-      </c>
-      <c r="P34" t="inlineStr">
-        <is>
-          <t>14:00</t>
-        </is>
-      </c>
-      <c r="Q34" t="inlineStr">
-        <is>
-          <t>Plumbing, Cleaning</t>
-        </is>
-      </c>
-      <c r="R34" t="inlineStr">
-        <is>
-          <t>#FBBC05</t>
-        </is>
-      </c>
+          <t>0424479524</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>789 Swanston Street, Melbourne VIC 3000</t>
+        </is>
+      </c>
+      <c r="G34" t="n">
+        <v>60</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2025-11-01 15:00</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>2025-11-01 16:00</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>Domestic Assistance</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>Domestic Assistance</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr"/>
+      <c r="N34" t="inlineStr"/>
+      <c r="O34" t="inlineStr"/>
+      <c r="P34" t="inlineStr"/>
+      <c r="Q34" t="inlineStr"/>
+      <c r="R34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2663,12 +2671,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>avery_allen</t>
+          <t>amelia_moore</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>avery.allen@example.com</t>
+          <t>amelia.moore@example.com</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -2678,40 +2686,40 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>0467264138</t>
+          <t>0441907220</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>605 Dohertys Road, Tarneit VIC 3029</t>
+          <t>123 Collins Street, Melbourne VIC 3000</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2025-11-01 08:00</t>
+          <t>2025-11-01 09:00</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>2025-11-01 10:00</t>
+          <t>2025-11-01 11:00</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Plumbing</t>
+          <t>Therapy Access</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Plumbing Issue</t>
+          <t>Therapy Access</t>
         </is>
       </c>
       <c r="M35" t="inlineStr"/>
@@ -2729,12 +2737,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>thomas_taylor</t>
+          <t>joseph_anderson</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>thomas.taylor@example.com</t>
+          <t>joseph.anderson@example.com</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -2744,40 +2752,40 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>0416270241</t>
+          <t>0463544454</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>170 Flinders Street, Melbourne VIC 3000</t>
+          <t>517 Ferntree Gully Road, Mulgrave VIC 3170</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2025-11-01 15:00</t>
+          <t>2025-11-01 08:00</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>2025-11-01 16:00</t>
+          <t>2025-11-01 09:00</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Life Skills Training</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>System Upgrade</t>
+          <t>Life Skills Training</t>
         </is>
       </c>
       <c r="M36" t="inlineStr"/>
@@ -2795,12 +2803,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>evelyn_thompson</t>
+          <t>william_hernandez</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>evelyn.thompson@example.com</t>
+          <t>william.hernandez@example.com</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -2810,12 +2818,12 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>0484495620</t>
+          <t>0482889093</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>842 Nicholson Street, Footscray VIC 3011</t>
+          <t>963 Acland Street, St Kilda VIC 3182</t>
         </is>
       </c>
       <c r="G37" t="n">
@@ -2823,27 +2831,27 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
+          <t>2025-11-01 09:00</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
           <t>2025-11-01 11:00</t>
         </is>
       </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>2025-11-01 13:00</t>
-        </is>
-      </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Community Access</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>High</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Gas Leak Repair</t>
+          <t>Community Access</t>
         </is>
       </c>
       <c r="M37" t="inlineStr"/>
@@ -2856,17 +2864,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Customer</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>paul_scott</t>
+          <t>tech_dakota</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>paul.scott@example.com</t>
+          <t>tech.dakota@company.com</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -2876,48 +2884,44 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>0429580246</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>595 Central Road, Clayton VIC 3168</t>
-        </is>
-      </c>
-      <c r="G38" t="n">
-        <v>120</v>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>2025-11-01 16:00</t>
-        </is>
-      </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>2025-11-01 18:00</t>
-        </is>
-      </c>
-      <c r="J38" t="inlineStr">
-        <is>
-          <t>Gas</t>
-        </is>
-      </c>
-      <c r="K38" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="L38" t="inlineStr">
-        <is>
-          <t>Gas Leak Repair</t>
-        </is>
-      </c>
-      <c r="M38" t="inlineStr"/>
-      <c r="N38" t="inlineStr"/>
-      <c r="O38" t="inlineStr"/>
-      <c r="P38" t="inlineStr"/>
-      <c r="Q38" t="inlineStr"/>
-      <c r="R38" t="inlineStr"/>
+          <t>0455237204</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr"/>
+      <c r="J38" t="inlineStr"/>
+      <c r="K38" t="inlineStr"/>
+      <c r="L38" t="inlineStr"/>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>290 Springvale Road, Mulgrave VIC 3170</t>
+        </is>
+      </c>
+      <c r="N38" t="n">
+        <v>6</v>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>06:00</t>
+        </is>
+      </c>
+      <c r="P38" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>Personal care, Domestic Assistance, Community Access</t>
+        </is>
+      </c>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>#FBBC05</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2927,12 +2931,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>emma_garcia</t>
+          <t>robert_rodriguez</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>emma.garcia@example.com</t>
+          <t>robert.rodriguez@example.com</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -2942,12 +2946,12 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>0453519669</t>
+          <t>0419304090</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>903 Springvale Road, Mulgrave VIC 3170</t>
+          <t>106 Springvale Road, Mulgrave VIC 3170</t>
         </is>
       </c>
       <c r="G39" t="n">
@@ -2955,27 +2959,27 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2025-11-01 09:00</t>
+          <t>2025-11-01 16:00</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>2025-11-01 11:00</t>
+          <t>2025-11-01 17:00</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Transport</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>System Upgrade</t>
+          <t>Transport</t>
         </is>
       </c>
       <c r="M39" t="inlineStr"/>
@@ -2988,17 +2992,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Customer</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>mary_johnson</t>
+          <t>tech_quinn</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>mary.johnson@example.com</t>
+          <t>tech.quinn@company.com</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -3008,63 +3012,59 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>0426130572</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>18 Acland Street, St Kilda VIC 3182</t>
-        </is>
-      </c>
-      <c r="G40" t="n">
-        <v>180</v>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>2025-11-01 16:00</t>
-        </is>
-      </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>2025-11-01 18:00</t>
-        </is>
-      </c>
-      <c r="J40" t="inlineStr">
-        <is>
-          <t>Gas</t>
-        </is>
-      </c>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="L40" t="inlineStr">
-        <is>
-          <t>Gas Leak Repair</t>
-        </is>
-      </c>
-      <c r="M40" t="inlineStr"/>
-      <c r="N40" t="inlineStr"/>
-      <c r="O40" t="inlineStr"/>
-      <c r="P40" t="inlineStr"/>
-      <c r="Q40" t="inlineStr"/>
-      <c r="R40" t="inlineStr"/>
+          <t>0440243301</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr"/>
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="inlineStr"/>
+      <c r="J40" t="inlineStr"/>
+      <c r="K40" t="inlineStr"/>
+      <c r="L40" t="inlineStr"/>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>15 Elizabeth Street, Melbourne VIC 3000</t>
+        </is>
+      </c>
+      <c r="N40" t="n">
+        <v>4</v>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="P40" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>Transport, Community Access, Therapy Access</t>
+        </is>
+      </c>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>#FF6D01</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Customer</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>tech_dakota</t>
+          <t>sophia_martinez</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>tech.dakota@company.com</t>
+          <t>sophia.martinez@example.com</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -3074,44 +3074,48 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>0428587579</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr"/>
-      <c r="G41" t="inlineStr"/>
-      <c r="H41" t="inlineStr"/>
-      <c r="I41" t="inlineStr"/>
-      <c r="J41" t="inlineStr"/>
-      <c r="K41" t="inlineStr"/>
-      <c r="L41" t="inlineStr"/>
-      <c r="M41" t="inlineStr">
-        <is>
-          <t>183 Bridge Road, Richmond VIC 3121</t>
-        </is>
-      </c>
-      <c r="N41" t="n">
-        <v>4</v>
-      </c>
-      <c r="O41" t="inlineStr">
-        <is>
-          <t>11:00</t>
-        </is>
-      </c>
-      <c r="P41" t="inlineStr">
-        <is>
-          <t>15:00</t>
-        </is>
-      </c>
-      <c r="Q41" t="inlineStr">
-        <is>
-          <t>HVAC, Plumbing</t>
-        </is>
-      </c>
-      <c r="R41" t="inlineStr">
-        <is>
-          <t>#FBBC05</t>
-        </is>
-      </c>
+          <t>0472304301</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>241 Chapel Street, South Yarra VIC 3141</t>
+        </is>
+      </c>
+      <c r="G41" t="n">
+        <v>60</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2025-11-01 08:00</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>2025-11-01 10:00</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>Therapy Access</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>Therapy Access</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr"/>
+      <c r="N41" t="inlineStr"/>
+      <c r="O41" t="inlineStr"/>
+      <c r="P41" t="inlineStr"/>
+      <c r="Q41" t="inlineStr"/>
+      <c r="R41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -3121,12 +3125,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>harper_martin</t>
+          <t>sarah_brown</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>harper.martin@example.com</t>
+          <t>sarah.brown@example.com</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -3136,40 +3140,40 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>0490505977</t>
+          <t>0456505373</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>865 Chapel Street, South Yarra VIC 3141</t>
+          <t>681 Princes Highway, Dandenong VIC 3175</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2025-11-01 08:00</t>
+          <t>2025-11-01 11:00</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>2025-11-01 10:00</t>
+          <t>2025-11-01 12:00</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Plumbing</t>
+          <t>Transport</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Emergency Callout</t>
+          <t>Transport</t>
         </is>
       </c>
       <c r="M42" t="inlineStr"/>
@@ -3187,12 +3191,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>donald_young</t>
+          <t>paul_scott</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>donald.young@example.com</t>
+          <t>paul.scott@example.com</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -3202,30 +3206,30 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>0446466682</t>
+          <t>0412734114</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>106 Nicholson Street, Footscray VIC 3011</t>
+          <t>88 Dandenong Road, Dandenong VIC 3175</t>
         </is>
       </c>
       <c r="G43" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>2025-11-01 16:00</t>
+          <t>2025-11-01 13:00</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>2025-11-01 18:00</t>
+          <t>2025-11-01 15:00</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Electric</t>
+          <t>Life Skills Training</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
@@ -3235,7 +3239,7 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Appliance Installation</t>
+          <t>Life Skills Training</t>
         </is>
       </c>
       <c r="M43" t="inlineStr"/>
@@ -3248,17 +3252,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Customer</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>tech_taylor</t>
+          <t>evelyn_thompson</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>tech.taylor@company.com</t>
+          <t>evelyn.thompson@example.com</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -3268,44 +3272,48 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>0484389248</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr"/>
-      <c r="G44" t="inlineStr"/>
-      <c r="H44" t="inlineStr"/>
-      <c r="I44" t="inlineStr"/>
-      <c r="J44" t="inlineStr"/>
-      <c r="K44" t="inlineStr"/>
-      <c r="L44" t="inlineStr"/>
-      <c r="M44" t="inlineStr">
-        <is>
-          <t>805 Commercial Road, South Yarra VIC 3141</t>
-        </is>
-      </c>
-      <c r="N44" t="n">
-        <v>4</v>
-      </c>
-      <c r="O44" t="inlineStr">
-        <is>
-          <t>12:00</t>
-        </is>
-      </c>
-      <c r="P44" t="inlineStr">
-        <is>
-          <t>16:00</t>
-        </is>
-      </c>
-      <c r="Q44" t="inlineStr">
-        <is>
-          <t>Solar, Electric, HVAC</t>
-        </is>
-      </c>
-      <c r="R44" t="inlineStr">
-        <is>
-          <t>#FBBC05</t>
-        </is>
-      </c>
+          <t>0473350201</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>456 Bourke Street, Melbourne VIC 3000</t>
+        </is>
+      </c>
+      <c r="G44" t="n">
+        <v>60</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2025-11-01 15:00</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>2025-11-01 16:00</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>Therapy Access</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>Therapy Access</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr"/>
+      <c r="N44" t="inlineStr"/>
+      <c r="O44" t="inlineStr"/>
+      <c r="P44" t="inlineStr"/>
+      <c r="Q44" t="inlineStr"/>
+      <c r="R44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -3315,12 +3323,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>daniel_white</t>
+          <t>james_miller</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>daniel.white@example.com</t>
+          <t>james.miller@example.com</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3330,40 +3338,40 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>0476768071</t>
+          <t>0493530298</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>637 Rathdowne Street, Carlton VIC 3053</t>
+          <t>89 Commercial Road, South Yarra VIC 3141</t>
         </is>
       </c>
       <c r="G45" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>2025-11-01 08:00</t>
+          <t>2025-11-01 12:00</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>2025-11-01 09:00</t>
+          <t>2025-11-01 13:00</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Electric</t>
+          <t>Community Access</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>High</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Electrical Fault</t>
+          <t>Community Access</t>
         </is>
       </c>
       <c r="M45" t="inlineStr"/>
@@ -3381,12 +3389,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>olivia_davis</t>
+          <t>charles_jackson</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>olivia.davis@example.com</t>
+          <t>charles.jackson@example.com</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3396,20 +3404,20 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>0433737847</t>
+          <t>0445934707</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>957 Clayton Campus, Monash University, Clayton VIC 3168</t>
+          <t>123 Collins Street, Melbourne VIC 3000</t>
         </is>
       </c>
       <c r="G46" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2025-11-01 10:00</t>
+          <t>2025-11-01 09:00</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
@@ -3419,17 +3427,17 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Electric</t>
+          <t>Domestic Assistance</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Maintenance Check</t>
+          <t>Domestic Assistance</t>
         </is>
       </c>
       <c r="M46" t="inlineStr"/>
@@ -3447,12 +3455,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>william_hernandez</t>
+          <t>avery_allen</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>william.hernandez@example.com</t>
+          <t>avery.allen@example.com</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -3462,40 +3470,40 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>0442165391</t>
+          <t>0430811406</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>682 Clayton Road, Clayton VIC 3168</t>
+          <t>88 Dandenong Road, Dandenong VIC 3175</t>
         </is>
       </c>
       <c r="G47" t="n">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="H47" t="inlineStr">
         <is>
+          <t>2025-11-01 13:00</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
           <t>2025-11-01 15:00</t>
         </is>
       </c>
-      <c r="I47" t="inlineStr">
-        <is>
-          <t>2025-11-01 16:00</t>
-        </is>
-      </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Plumbing</t>
+          <t>Life Skills Training</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Plumbing Issue</t>
+          <t>Life Skills Training</t>
         </is>
       </c>
       <c r="M47" t="inlineStr"/>
@@ -3508,17 +3516,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Customer</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>david_williams</t>
+          <t>tech_sage</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>david.williams@example.com</t>
+          <t>tech.sage@company.com</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -3528,48 +3536,44 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>0427779725</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>552 Dandenong Railway Station, Dandenong VIC 3175</t>
-        </is>
-      </c>
-      <c r="G48" t="n">
-        <v>90</v>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>2025-11-01 09:00</t>
-        </is>
-      </c>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>2025-11-01 11:00</t>
-        </is>
-      </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>Electric</t>
-        </is>
-      </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="L48" t="inlineStr">
-        <is>
-          <t>Maintenance Check</t>
-        </is>
-      </c>
-      <c r="M48" t="inlineStr"/>
-      <c r="N48" t="inlineStr"/>
-      <c r="O48" t="inlineStr"/>
-      <c r="P48" t="inlineStr"/>
-      <c r="Q48" t="inlineStr"/>
-      <c r="R48" t="inlineStr"/>
+          <t>0464281145</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr"/>
+      <c r="G48" t="inlineStr"/>
+      <c r="H48" t="inlineStr"/>
+      <c r="I48" t="inlineStr"/>
+      <c r="J48" t="inlineStr"/>
+      <c r="K48" t="inlineStr"/>
+      <c r="L48" t="inlineStr"/>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>140 Dandenong Railway Station, Dandenong VIC 3175</t>
+        </is>
+      </c>
+      <c r="N48" t="n">
+        <v>4</v>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="P48" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>Transport, Community Access</t>
+        </is>
+      </c>
+      <c r="R48" t="inlineStr">
+        <is>
+          <t>#4285F4</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -3579,12 +3583,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>tech_drew</t>
+          <t>tech_blake</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>tech.drew@company.com</t>
+          <t>tech.blake@company.com</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -3594,7 +3598,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>0428989390</t>
+          <t>0470755682</t>
         </is>
       </c>
       <c r="F49" t="inlineStr"/>
@@ -3606,7 +3610,7 @@
       <c r="L49" t="inlineStr"/>
       <c r="M49" t="inlineStr">
         <is>
-          <t>531 Ferntree Gully Road, Mulgrave VIC 3170</t>
+          <t>951 Ferntree Gully Road, Mulgrave VIC 3170</t>
         </is>
       </c>
       <c r="N49" t="n">
@@ -3614,39 +3618,39 @@
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="Q49" t="inlineStr">
         <is>
-          <t>IT, Electric</t>
+          <t>Personal care, Domestic Assistance, Life Skills Training</t>
         </is>
       </c>
       <c r="R49" t="inlineStr">
         <is>
-          <t>#4285F4</t>
+          <t>#34A853</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Customer</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>sophia_martinez</t>
+          <t>tech_cameron</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>sophia.martinez@example.com</t>
+          <t>tech.cameron@company.com</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -3656,48 +3660,44 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>0476632499</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>484 Elizabeth Street, Melbourne VIC 3000</t>
-        </is>
-      </c>
-      <c r="G50" t="n">
-        <v>120</v>
-      </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>2025-11-01 16:00</t>
-        </is>
-      </c>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>2025-11-01 18:00</t>
-        </is>
-      </c>
-      <c r="J50" t="inlineStr">
-        <is>
-          <t>Electric</t>
-        </is>
-      </c>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="L50" t="inlineStr">
-        <is>
-          <t>Maintenance Check</t>
-        </is>
-      </c>
-      <c r="M50" t="inlineStr"/>
-      <c r="N50" t="inlineStr"/>
-      <c r="O50" t="inlineStr"/>
-      <c r="P50" t="inlineStr"/>
-      <c r="Q50" t="inlineStr"/>
-      <c r="R50" t="inlineStr"/>
+          <t>0419244027</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr"/>
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="inlineStr"/>
+      <c r="K50" t="inlineStr"/>
+      <c r="L50" t="inlineStr"/>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>501 Nicholson Street, Footscray VIC 3011</t>
+        </is>
+      </c>
+      <c r="N50" t="n">
+        <v>8</v>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="P50" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>Personal care, Domestic Assistance, Community Access</t>
+        </is>
+      </c>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>#FF6D01</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -3707,12 +3707,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>michael_jones</t>
+          <t>richard_gonzalez</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>michael.jones@example.com</t>
+          <t>richard.gonzalez@example.com</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -3722,40 +3722,40 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>0475007409</t>
+          <t>0472941372</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>986 Ferntree Gully Road, Mulgrave VIC 3170</t>
+          <t>119 Swanston Street, Melbourne VIC 3000</t>
         </is>
       </c>
       <c r="G51" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>2025-11-01 11:00</t>
+          <t>2025-11-01 13:00</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>2025-11-01 12:00</t>
+          <t>2025-11-01 15:00</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Plumbing</t>
+          <t>Life Skills Training</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Plumbing Issue</t>
+          <t>Life Skills Training</t>
         </is>
       </c>
       <c r="M51" t="inlineStr"/>

</xml_diff>